<commit_message>
proposal and start introduction
</commit_message>
<xml_diff>
--- a/literature-review.xlsx
+++ b/literature-review.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pasca\Documents\School\TCS\Year 3\Research Project\llm-triage-automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C767A785-2969-42E3-BCD5-5259FFA4260A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A8EB14A-1A02-404A-97F7-F4F0D423F5C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CC14483C-FFA5-42D2-83F7-E08FD9CC60FC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="95">
   <si>
     <t>Keywords</t>
   </si>
@@ -285,6 +285,42 @@
   </si>
   <si>
     <t>Deep learning for automated triaging of 4581 breast MRI examinations from the DENSE trial</t>
+  </si>
+  <si>
+    <t>CySecBERT: A Domain-Adapted Language Model for the Cybersecurity Domain</t>
+  </si>
+  <si>
+    <t>large language model cybersecurity</t>
+  </si>
+  <si>
+    <t>Securebert: A domain-specific language model for cybersecurity</t>
+  </si>
+  <si>
+    <t>Cybert: Cybersecurity claim classification by fine-tuning the bert language model</t>
+  </si>
+  <si>
+    <t>Cybert: Contextualized embeddings for the cybersecurity domain</t>
+  </si>
+  <si>
+    <t>Generative AI and Large Language Modeling in Cybersecurity</t>
+  </si>
+  <si>
+    <t>Assessing Cybersecurity Vulnerabilities in Code Large Language Models</t>
+  </si>
+  <si>
+    <t>Large Language Models in Cybersecurity: State-of-the-Art</t>
+  </si>
+  <si>
+    <t>CyberSecEval 2: A Wide-Ranging Cybersecurity Evaluation Suite for Large Language Models</t>
+  </si>
+  <si>
+    <t>What are the latest cybersecurity trends? a case study grounded in language models</t>
+  </si>
+  <si>
+    <t>Using large language models for cybersecurity capture-the-flag challenges and certification questions</t>
+  </si>
+  <si>
+    <t>AI, ML, AND LARGE LANGUAGE MODELS IN CYBERSECURITY</t>
   </si>
 </sst>
 </file>
@@ -355,18 +391,11 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
           <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -381,13 +410,6 @@
       <fill>
         <patternFill>
           <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -701,10 +723,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA56E3F7-3E01-4BDD-85F3-CABBFCE5FF08}">
-  <dimension ref="A1:H69"/>
+  <dimension ref="A1:H80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1350,7 +1372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C65" t="s">
         <v>79</v>
       </c>
@@ -1358,7 +1380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C66" t="s">
         <v>41</v>
       </c>
@@ -1366,7 +1388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C67" t="s">
         <v>80</v>
       </c>
@@ -1374,7 +1396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C68" t="s">
         <v>81</v>
       </c>
@@ -1382,7 +1404,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C69" t="s">
         <v>82</v>
       </c>
@@ -1390,13 +1412,112 @@
         <v>0</v>
       </c>
     </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>84</v>
+      </c>
+      <c r="B70">
+        <v>119000</v>
+      </c>
+      <c r="C70" t="s">
+        <v>83</v>
+      </c>
+      <c r="D70" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C71" t="s">
+        <v>85</v>
+      </c>
+      <c r="D71" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C72" t="s">
+        <v>86</v>
+      </c>
+      <c r="D72" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C73" t="s">
+        <v>87</v>
+      </c>
+      <c r="D73" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C74" t="s">
+        <v>88</v>
+      </c>
+      <c r="D74" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C75" t="s">
+        <v>89</v>
+      </c>
+      <c r="D75" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C76" t="s">
+        <v>90</v>
+      </c>
+      <c r="D76" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C77" t="s">
+        <v>91</v>
+      </c>
+      <c r="D77" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C78" t="s">
+        <v>92</v>
+      </c>
+      <c r="D78" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C79" t="s">
+        <v>93</v>
+      </c>
+      <c r="D79" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C80" t="s">
+        <v>94</v>
+      </c>
+      <c r="D80" t="b">
+        <v>1</v>
+      </c>
+      <c r="E80" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A46:XFD1048576 B45:XFD45 A1:XFD20 A21:E21 G21:XFD21 A22:XFD44">
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="TRUE">
+  <conditionalFormatting sqref="A1:XFD20 A21:E21 G21:XFD21 A22:XFD44 B45:XFD45 A46:XFD1048576">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",A1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:XFD20 G21:XFD21 A22:XFD44 B45:XFD45 A46:XFD1048576 A21:E21">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",A1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H1048576">

</xml_diff>

<commit_message>
methodologies, planning and use of ai
</commit_message>
<xml_diff>
--- a/literature-review.xlsx
+++ b/literature-review.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pasca\Documents\School\TCS\Year 3\Research Project\llm-triage-automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9CF7362-C37F-40A8-8F67-1A042C0B1E69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{520FC637-22D3-4B05-8A5C-8CB098192432}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CC14483C-FFA5-42D2-83F7-E08FD9CC60FC}"/>
   </bookViews>
@@ -781,8 +781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA56E3F7-3E01-4BDD-85F3-CABBFCE5FF08}">
   <dimension ref="A1:H84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="C65" sqref="C65"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1473,7 +1473,7 @@
       <c r="B69">
         <v>119000</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C69" s="4" t="s">
         <v>83</v>
       </c>
       <c r="D69" t="b">
@@ -1501,7 +1501,7 @@
         <v>87</v>
       </c>
       <c r="D72" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
@@ -1553,7 +1553,7 @@
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C79" t="s">
+      <c r="C79" s="4" t="s">
         <v>94</v>
       </c>
       <c r="D79" t="b">

</xml_diff>